<commit_message>
Refactor Code containing duplicates
</commit_message>
<xml_diff>
--- a/Employee_Data.xlsx
+++ b/Employee_Data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mario\Documents\VSC\TAF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mario\Documents\VSC\TAF\PythonSQL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A8BEEFE-6F09-47C6-B5C3-DF184F335AD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA8E9976-5198-4F69-8485-855DB19B6B9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,9 +25,6 @@
     <t xml:space="preserve">John </t>
   </si>
   <si>
-    <t xml:space="preserve">Doe </t>
-  </si>
-  <si>
     <t xml:space="preserve">john.doe@email.com </t>
   </si>
   <si>
@@ -68,6 +65,9 @@
   </si>
   <si>
     <t>Finance</t>
+  </si>
+  <si>
+    <t>Doe</t>
   </si>
 </sst>
 </file>
@@ -338,7 +338,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E3"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -351,10 +351,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
       </c>
       <c r="D1" s="4">
         <v>1234567890</v>
@@ -363,27 +363,27 @@
         <v>45301</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G1" s="3">
         <v>70000</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="D2" s="4">
         <v>987654321</v>
@@ -392,27 +392,27 @@
         <v>45099</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G2" s="3">
         <v>90000</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="D3" s="4">
         <v>1231231234</v>
@@ -421,13 +421,13 @@
         <v>44818</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G3" s="3">
         <v>65000</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I3" s="1">
         <v>2</v>

</xml_diff>

<commit_message>
Adjusted insertation to references manager's email
</commit_message>
<xml_diff>
--- a/Employee_Data.xlsx
+++ b/Employee_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mario\Documents\VSC\TAF\PythonSQL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA8E9976-5198-4F69-8485-855DB19B6B9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87C0DEF5-95E1-4322-A106-13F7AE25CE9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21720" yWindow="2610" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t xml:space="preserve">John </t>
   </si>
@@ -338,7 +338,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -429,8 +429,8 @@
       <c r="H3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="1">
-        <v>2</v>
+      <c r="I3" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adjusted data insertation to skipped Already included Data
</commit_message>
<xml_diff>
--- a/Employee_Data.xlsx
+++ b/Employee_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mario\Documents\VSC\TAF\PythonSQL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87C0DEF5-95E1-4322-A106-13F7AE25CE9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28A195D4-2ED2-439B-BC21-25928C9D5D8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-21720" yWindow="2610" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
-  <si>
-    <t xml:space="preserve">John </t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
     <t xml:space="preserve">john.doe@email.com </t>
   </si>
@@ -68,6 +65,18 @@
   </si>
   <si>
     <t>Doe</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Aaron</t>
+  </si>
+  <si>
+    <t>Ho</t>
+  </si>
+  <si>
+    <t>aaron.ho@email.com</t>
   </si>
 </sst>
 </file>
@@ -77,7 +86,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -88,6 +97,13 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -111,12 +127,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -335,26 +354,28 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="19.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" style="5"/>
+    <col min="7" max="7" width="12.5703125" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
       </c>
       <c r="D1" s="4">
         <v>1234567890</v>
@@ -363,27 +384,27 @@
         <v>45301</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G1" s="3">
         <v>70000</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="D2" s="4">
         <v>987654321</v>
@@ -392,27 +413,27 @@
         <v>45099</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G2" s="3">
         <v>90000</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="D3" s="4">
         <v>1231231234</v>
@@ -421,19 +442,49 @@
         <v>44818</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G3" s="3">
         <v>65000</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="4">
+        <v>4444444444</v>
+      </c>
+      <c r="E4" s="2">
+        <v>45371</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="6">
+        <v>70000</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>